<commit_message>
Fixed bugs related to wiring of one level chains and leaf-to-root chain reversing. Updated scaffold components
</commit_message>
<xml_diff>
--- a/test/excel/Too-map-D.xlsx
+++ b/test/excel/Too-map-D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>B. de Bono &amp; N. Kokash</t>
   </si>
   <si>
-    <t>2021-06-24</t>
-  </si>
-  <si>
     <t>layout</t>
   </si>
   <si>
@@ -152,6 +149,12 @@
     <t>arcCenter</t>
   </si>
   <si>
+    <t>controlPoint</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
     <t>w-L-P</t>
   </si>
   <si>
@@ -216,6 +219,18 @@
   </si>
   <si>
     <t>#800080</t>
+  </si>
+  <si>
+    <t>w-S-Y</t>
+  </si>
+  <si>
+    <t>Systemic pre-lymphatic venous</t>
+  </si>
+  <si>
+    <t>w-Y-P</t>
+  </si>
+  <si>
+    <t>Systemic post-lymphatic venous</t>
   </si>
   <si>
     <t>facets</t>
@@ -654,9 +669,7 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -685,135 +698,135 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.8</v>
+      <c r="F10" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -842,227 +855,279 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
+      <c r="I1" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G11" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1092,33 +1157,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1128,16 +1193,16 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1147,16 +1212,16 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1166,16 +1231,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1185,19 +1250,19 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1223,21 +1288,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#54 chore: pulled latest from open-physiology-viewer/open-physiology-viewer & resolved merge conflicts
</commit_message>
<xml_diff>
--- a/test/excel/Too-map-D.xlsx
+++ b/test/excel/Too-map-D.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>B. de Bono &amp; N. Kokash</t>
   </si>
   <si>
-    <t>2021-06-24</t>
-  </si>
-  <si>
     <t>layout</t>
   </si>
   <si>
@@ -152,6 +149,12 @@
     <t>arcCenter</t>
   </si>
   <si>
+    <t>controlPoint</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
     <t>w-L-P</t>
   </si>
   <si>
@@ -216,6 +219,18 @@
   </si>
   <si>
     <t>#800080</t>
+  </si>
+  <si>
+    <t>w-S-Y</t>
+  </si>
+  <si>
+    <t>Systemic pre-lymphatic venous</t>
+  </si>
+  <si>
+    <t>w-Y-P</t>
+  </si>
+  <si>
+    <t>Systemic post-lymphatic venous</t>
   </si>
   <si>
     <t>facets</t>
@@ -654,9 +669,7 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -685,135 +698,135 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.8</v>
+      <c r="F10" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -842,227 +855,279 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
+      <c r="I1" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G11" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1092,33 +1157,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1128,16 +1193,16 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1147,16 +1212,16 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1166,16 +1231,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1185,19 +1250,19 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1223,21 +1288,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>